<commit_message>
changing test case type to add language info in test case for research screens
</commit_message>
<xml_diff>
--- a/tm/tm.service/src/test/resources/batchimport/testcase/import-incorrect-scripted-tc.xlsx
+++ b/tm/tm.service/src/test/resources/batchimport/testcase/import-incorrect-scripted-tc.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="57">
   <si>
     <t>ACTION</t>
   </si>
@@ -187,9 +187,6 @@
   </si>
   <si>
     <t>TC_SCRIPT</t>
-  </si>
-  <si>
-    <t>SCRIPTED</t>
   </si>
   <si>
     <t>Feature: Make something</t>
@@ -661,8 +658,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="W10" sqref="W10"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="X5" sqref="X5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -823,13 +820,13 @@
       <c r="V2" s="2"/>
       <c r="W2" s="2"/>
       <c r="X2" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y2" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="Z2" s="2" t="s">
         <v>55</v>
-      </c>
-      <c r="Y2" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="Z2" s="2" t="s">
-        <v>56</v>
       </c>
       <c r="AA2" s="2"/>
       <c r="AB2" s="2"/>

</xml_diff>